<commit_message>
sirajganj sadar excel file updated
</commit_message>
<xml_diff>
--- a/shirajganj_kazipur.xlsx
+++ b/shirajganj_kazipur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tawsif/Downloads/csv-to-pdf-final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AC7C604-3690-9240-A5E7-4AD4059A903D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2562A9-D825-FE4D-A184-54CB44A0593A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9440" yWindow="0" windowWidth="24400" windowHeight="21000" xr2:uid="{4B0A96A3-5DBC-704A-805C-C63247901FE7}"/>
   </bookViews>
@@ -1402,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2704D1E-A6BE-954D-930C-42043A0C7FD3}">
   <dimension ref="A1:G390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G390"/>
     </sheetView>
   </sheetViews>
@@ -1412,7 +1412,7 @@
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="35.33203125" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
-    <col min="7" max="7" width="61.33203125" customWidth="1"/>
+    <col min="7" max="7" width="45.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17">

</xml_diff>